<commit_message>
allow filtering of wss categories
</commit_message>
<xml_diff>
--- a/conf/csvImport/SW Files/SW Files/New Probcodes.xlsx
+++ b/conf/csvImport/SW Files/SW Files/New Probcodes.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27610"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbaird/Desktop/SW Files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Shared Directory/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13360" yWindow="500" windowWidth="24420" windowHeight="21060"/>
+    <workbookView xWindow="1180" yWindow="460" windowWidth="24420" windowHeight="13940"/>
   </bookViews>
   <sheets>
     <sheet name="probcode" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="191">
   <si>
     <t>Account</t>
   </si>
@@ -598,16 +598,38 @@
   </si>
   <si>
     <t>STO1</t>
+  </si>
+  <si>
+    <t>OFFice 365</t>
+  </si>
+  <si>
+    <t>Network</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -630,13 +652,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -949,11 +975,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F81"/>
+  <dimension ref="A1:F96"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H1" sqref="H1:H1048576"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D26" sqref="A1:F96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -991,25 +1017,19 @@
       <c r="B2" t="s">
         <v>175</v>
       </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>175</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -1019,12 +1039,6 @@
       <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -1034,10 +1048,10 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>176</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -1048,10 +1062,10 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>172</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -1062,10 +1076,10 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
+        <v>176</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -1076,10 +1090,10 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
+        <v>172</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -1090,10 +1104,10 @@
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -1104,38 +1118,38 @@
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D10" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D11" t="s">
-        <v>177</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -1145,12 +1159,6 @@
       <c r="B13" t="s">
         <v>21</v>
       </c>
-      <c r="C13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" t="s">
-        <v>178</v>
-      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -1160,10 +1168,10 @@
         <v>21</v>
       </c>
       <c r="C14" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D14" t="s">
-        <v>26</v>
+        <v>177</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -1174,10 +1182,10 @@
         <v>21</v>
       </c>
       <c r="C15" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D15" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -1188,10 +1196,10 @@
         <v>21</v>
       </c>
       <c r="C16" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D16" t="s">
-        <v>29</v>
+        <v>178</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -1202,10 +1210,10 @@
         <v>21</v>
       </c>
       <c r="C17" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D17" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -1216,10 +1224,10 @@
         <v>21</v>
       </c>
       <c r="C18" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D18" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -1230,10 +1238,10 @@
         <v>21</v>
       </c>
       <c r="C19" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D19" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -1244,10 +1252,10 @@
         <v>21</v>
       </c>
       <c r="C20" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D20" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -1258,10 +1266,10 @@
         <v>21</v>
       </c>
       <c r="C21" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D21" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -1272,10 +1280,10 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D22" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -1286,16 +1294,10 @@
         <v>21</v>
       </c>
       <c r="C23" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D23" t="s">
-        <v>44</v>
-      </c>
-      <c r="E23" t="s">
-        <v>43</v>
-      </c>
-      <c r="F23" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -1306,16 +1308,10 @@
         <v>21</v>
       </c>
       <c r="C24" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D24" t="s">
-        <v>44</v>
-      </c>
-      <c r="E24" t="s">
-        <v>46</v>
-      </c>
-      <c r="F24" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -1326,16 +1322,10 @@
         <v>21</v>
       </c>
       <c r="C25" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D25" t="s">
-        <v>44</v>
-      </c>
-      <c r="E25" t="s">
-        <v>48</v>
-      </c>
-      <c r="F25" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -1346,17 +1336,11 @@
         <v>21</v>
       </c>
       <c r="C26" t="s">
-        <v>42</v>
+        <v>189</v>
       </c>
       <c r="D26" t="s">
         <v>44</v>
       </c>
-      <c r="E26" t="s">
-        <v>50</v>
-      </c>
-      <c r="F26" t="s">
-        <v>51</v>
-      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
@@ -1372,10 +1356,10 @@
         <v>44</v>
       </c>
       <c r="E27" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="F27" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -1392,10 +1376,10 @@
         <v>44</v>
       </c>
       <c r="E28" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="F28" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -1412,10 +1396,10 @@
         <v>44</v>
       </c>
       <c r="E29" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="F29" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -1426,10 +1410,16 @@
         <v>21</v>
       </c>
       <c r="C30" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="D30" t="s">
-        <v>59</v>
+        <v>44</v>
+      </c>
+      <c r="E30" t="s">
+        <v>50</v>
+      </c>
+      <c r="F30" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -1440,10 +1430,16 @@
         <v>21</v>
       </c>
       <c r="C31" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="D31" t="s">
-        <v>61</v>
+        <v>44</v>
+      </c>
+      <c r="E31" t="s">
+        <v>52</v>
+      </c>
+      <c r="F31" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -1454,10 +1450,16 @@
         <v>21</v>
       </c>
       <c r="C32" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="D32" t="s">
-        <v>63</v>
+        <v>44</v>
+      </c>
+      <c r="E32" t="s">
+        <v>54</v>
+      </c>
+      <c r="F32" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -1468,10 +1470,16 @@
         <v>21</v>
       </c>
       <c r="C33" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="D33" t="s">
-        <v>65</v>
+        <v>44</v>
+      </c>
+      <c r="E33" t="s">
+        <v>56</v>
+      </c>
+      <c r="F33" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -1482,10 +1490,10 @@
         <v>21</v>
       </c>
       <c r="C34" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D34" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -1496,10 +1504,10 @@
         <v>21</v>
       </c>
       <c r="C35" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="D35" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -1510,10 +1518,10 @@
         <v>21</v>
       </c>
       <c r="C36" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="D36" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
@@ -1524,10 +1532,10 @@
         <v>21</v>
       </c>
       <c r="C37" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D37" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -1538,10 +1546,10 @@
         <v>21</v>
       </c>
       <c r="C38" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="D38" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -1552,10 +1560,10 @@
         <v>21</v>
       </c>
       <c r="C39" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="D39" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
@@ -1566,10 +1574,10 @@
         <v>21</v>
       </c>
       <c r="C40" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="D40" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
@@ -1580,10 +1588,10 @@
         <v>21</v>
       </c>
       <c r="C41" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D41" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
@@ -1594,10 +1602,10 @@
         <v>21</v>
       </c>
       <c r="C42" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="D42" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
@@ -1608,10 +1616,10 @@
         <v>21</v>
       </c>
       <c r="C43" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="D43" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
@@ -1622,10 +1630,10 @@
         <v>21</v>
       </c>
       <c r="C44" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="D44" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
@@ -1636,84 +1644,66 @@
         <v>21</v>
       </c>
       <c r="C45" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="D45" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>89</v>
+        <v>19</v>
       </c>
       <c r="B46" t="s">
-        <v>92</v>
+        <v>21</v>
       </c>
       <c r="C46" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="D46" t="s">
-        <v>93</v>
-      </c>
-      <c r="E46" t="s">
-        <v>91</v>
-      </c>
-      <c r="F46" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>89</v>
+        <v>19</v>
       </c>
       <c r="B47" t="s">
-        <v>92</v>
+        <v>21</v>
       </c>
       <c r="C47" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="D47" t="s">
-        <v>93</v>
-      </c>
-      <c r="E47" t="s">
-        <v>95</v>
-      </c>
-      <c r="F47" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>89</v>
+        <v>19</v>
       </c>
       <c r="B48" t="s">
-        <v>92</v>
+        <v>21</v>
       </c>
       <c r="C48" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D48" t="s">
-        <v>93</v>
-      </c>
-      <c r="E48" t="s">
-        <v>97</v>
-      </c>
-      <c r="F48" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>89</v>
+        <v>19</v>
       </c>
       <c r="B49" t="s">
-        <v>92</v>
+        <v>21</v>
       </c>
       <c r="C49" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="D49" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
@@ -1723,12 +1713,6 @@
       <c r="B50" t="s">
         <v>92</v>
       </c>
-      <c r="C50" t="s">
-        <v>101</v>
-      </c>
-      <c r="D50" t="s">
-        <v>102</v>
-      </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
@@ -1738,16 +1722,10 @@
         <v>92</v>
       </c>
       <c r="C51" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="D51" t="s">
-        <v>105</v>
-      </c>
-      <c r="E51" t="s">
-        <v>104</v>
-      </c>
-      <c r="F51" t="s">
-        <v>181</v>
+        <v>93</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
@@ -1758,16 +1736,16 @@
         <v>92</v>
       </c>
       <c r="C52" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="D52" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="E52" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="F52" t="s">
-        <v>182</v>
+        <v>94</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
@@ -1778,16 +1756,16 @@
         <v>92</v>
       </c>
       <c r="C53" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="D53" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="E53" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="F53" t="s">
-        <v>183</v>
+        <v>96</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
@@ -1798,16 +1776,16 @@
         <v>92</v>
       </c>
       <c r="C54" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="D54" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="E54" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="F54" t="s">
-        <v>184</v>
+        <v>98</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
@@ -1818,10 +1796,10 @@
         <v>92</v>
       </c>
       <c r="C55" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="D55" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
@@ -1832,10 +1810,10 @@
         <v>92</v>
       </c>
       <c r="C56" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="D56" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
@@ -1846,10 +1824,10 @@
         <v>92</v>
       </c>
       <c r="C57" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="D57" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
@@ -1860,10 +1838,16 @@
         <v>92</v>
       </c>
       <c r="C58" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="D58" t="s">
-        <v>116</v>
+        <v>105</v>
+      </c>
+      <c r="E58" t="s">
+        <v>104</v>
+      </c>
+      <c r="F58" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
@@ -1874,10 +1858,16 @@
         <v>92</v>
       </c>
       <c r="C59" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="D59" t="s">
-        <v>118</v>
+        <v>105</v>
+      </c>
+      <c r="E59" t="s">
+        <v>106</v>
+      </c>
+      <c r="F59" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
@@ -1888,10 +1878,16 @@
         <v>92</v>
       </c>
       <c r="C60" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="D60" t="s">
-        <v>120</v>
+        <v>105</v>
+      </c>
+      <c r="E60" t="s">
+        <v>107</v>
+      </c>
+      <c r="F60" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
@@ -1902,198 +1898,150 @@
         <v>92</v>
       </c>
       <c r="C61" t="s">
-        <v>121</v>
+        <v>103</v>
       </c>
       <c r="D61" t="s">
-        <v>122</v>
+        <v>105</v>
+      </c>
+      <c r="E61" t="s">
+        <v>108</v>
+      </c>
+      <c r="F61" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>123</v>
+        <v>89</v>
       </c>
       <c r="B62" t="s">
-        <v>125</v>
+        <v>92</v>
       </c>
       <c r="C62" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="D62" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>123</v>
+        <v>89</v>
       </c>
       <c r="B63" t="s">
-        <v>125</v>
+        <v>92</v>
       </c>
       <c r="C63" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="D63" t="s">
-        <v>179</v>
+        <v>112</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>128</v>
+        <v>89</v>
       </c>
       <c r="B64" t="s">
-        <v>130</v>
+        <v>92</v>
       </c>
       <c r="C64" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
       <c r="D64" t="s">
-        <v>180</v>
-      </c>
-      <c r="E64" t="s">
-        <v>185</v>
-      </c>
-      <c r="F64" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>128</v>
+        <v>89</v>
       </c>
       <c r="B65" t="s">
-        <v>130</v>
+        <v>92</v>
       </c>
       <c r="C65" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="D65" t="s">
-        <v>187</v>
-      </c>
-      <c r="E65" t="s">
-        <v>186</v>
-      </c>
-      <c r="F65" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>128</v>
+        <v>89</v>
       </c>
       <c r="B66" t="s">
-        <v>130</v>
+        <v>92</v>
       </c>
       <c r="C66" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="D66" t="s">
-        <v>187</v>
-      </c>
-      <c r="E66" t="s">
-        <v>134</v>
-      </c>
-      <c r="F66" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>128</v>
+        <v>89</v>
       </c>
       <c r="B67" t="s">
-        <v>130</v>
+        <v>92</v>
       </c>
       <c r="C67" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="D67" t="s">
-        <v>187</v>
-      </c>
-      <c r="E67" t="s">
-        <v>136</v>
-      </c>
-      <c r="F67" t="s">
-        <v>174</v>
+        <v>120</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>128</v>
+        <v>89</v>
       </c>
       <c r="B68" t="s">
-        <v>130</v>
+        <v>92</v>
       </c>
       <c r="C68" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D68" t="s">
-        <v>187</v>
-      </c>
-      <c r="E68" t="s">
-        <v>137</v>
-      </c>
-      <c r="F68" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B69" t="s">
-        <v>130</v>
-      </c>
-      <c r="C69" t="s">
-        <v>132</v>
-      </c>
-      <c r="D69" t="s">
-        <v>187</v>
-      </c>
-      <c r="E69" t="s">
-        <v>138</v>
-      </c>
-      <c r="F69" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B70" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C70" t="s">
-        <v>11</v>
+        <v>124</v>
       </c>
       <c r="D70" t="s">
-        <v>141</v>
-      </c>
-      <c r="E70" t="s">
-        <v>140</v>
-      </c>
-      <c r="F70" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B71" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C71" t="s">
-        <v>11</v>
+        <v>127</v>
       </c>
       <c r="D71" t="s">
-        <v>141</v>
-      </c>
-      <c r="E71" t="s">
-        <v>143</v>
-      </c>
-      <c r="F71" t="s">
-        <v>144</v>
+        <v>179</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
@@ -2103,18 +2051,6 @@
       <c r="B72" t="s">
         <v>130</v>
       </c>
-      <c r="C72" t="s">
-        <v>11</v>
-      </c>
-      <c r="D72" t="s">
-        <v>141</v>
-      </c>
-      <c r="E72" t="s">
-        <v>145</v>
-      </c>
-      <c r="F72" t="s">
-        <v>146</v>
-      </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
@@ -2124,16 +2060,10 @@
         <v>130</v>
       </c>
       <c r="C73" t="s">
-        <v>13</v>
+        <v>129</v>
       </c>
       <c r="D73" t="s">
-        <v>188</v>
-      </c>
-      <c r="E73" t="s">
-        <v>147</v>
-      </c>
-      <c r="F73" t="s">
-        <v>148</v>
+        <v>180</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
@@ -2144,16 +2074,16 @@
         <v>130</v>
       </c>
       <c r="C74" t="s">
-        <v>13</v>
+        <v>129</v>
       </c>
       <c r="D74" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="E74" t="s">
-        <v>149</v>
+        <v>185</v>
       </c>
       <c r="F74" t="s">
-        <v>150</v>
+        <v>131</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
@@ -2164,16 +2094,10 @@
         <v>130</v>
       </c>
       <c r="C75" t="s">
-        <v>13</v>
+        <v>190</v>
       </c>
       <c r="D75" t="s">
-        <v>188</v>
-      </c>
-      <c r="E75" t="s">
-        <v>145</v>
-      </c>
-      <c r="F75" t="s">
-        <v>151</v>
+        <v>187</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
@@ -2184,16 +2108,16 @@
         <v>130</v>
       </c>
       <c r="C76" t="s">
-        <v>152</v>
+        <v>132</v>
       </c>
       <c r="D76" t="s">
-        <v>154</v>
+        <v>187</v>
       </c>
       <c r="E76" t="s">
-        <v>153</v>
+        <v>186</v>
       </c>
       <c r="F76" t="s">
-        <v>155</v>
+        <v>133</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
@@ -2204,16 +2128,16 @@
         <v>130</v>
       </c>
       <c r="C77" t="s">
-        <v>152</v>
+        <v>132</v>
       </c>
       <c r="D77" t="s">
-        <v>154</v>
+        <v>187</v>
       </c>
       <c r="E77" t="s">
-        <v>156</v>
+        <v>134</v>
       </c>
       <c r="F77" t="s">
-        <v>157</v>
+        <v>135</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
@@ -2224,16 +2148,16 @@
         <v>130</v>
       </c>
       <c r="C78" t="s">
-        <v>152</v>
+        <v>132</v>
       </c>
       <c r="D78" t="s">
-        <v>154</v>
+        <v>187</v>
       </c>
       <c r="E78" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="F78" t="s">
-        <v>158</v>
+        <v>174</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
@@ -2244,16 +2168,16 @@
         <v>130</v>
       </c>
       <c r="C79" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="D79" t="s">
-        <v>173</v>
+        <v>187</v>
       </c>
       <c r="E79" t="s">
-        <v>160</v>
+        <v>137</v>
       </c>
       <c r="F79" t="s">
-        <v>161</v>
+        <v>137</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
@@ -2264,16 +2188,16 @@
         <v>130</v>
       </c>
       <c r="C80" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="D80" t="s">
-        <v>173</v>
+        <v>187</v>
       </c>
       <c r="E80" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="F80" t="s">
-        <v>163</v>
+        <v>139</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
@@ -2284,15 +2208,291 @@
         <v>130</v>
       </c>
       <c r="C81" t="s">
+        <v>11</v>
+      </c>
+      <c r="D81" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>128</v>
+      </c>
+      <c r="B82" t="s">
+        <v>130</v>
+      </c>
+      <c r="C82" t="s">
+        <v>11</v>
+      </c>
+      <c r="D82" t="s">
+        <v>141</v>
+      </c>
+      <c r="E82" t="s">
+        <v>140</v>
+      </c>
+      <c r="F82" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>128</v>
+      </c>
+      <c r="B83" t="s">
+        <v>130</v>
+      </c>
+      <c r="C83" t="s">
+        <v>11</v>
+      </c>
+      <c r="D83" t="s">
+        <v>141</v>
+      </c>
+      <c r="E83" t="s">
+        <v>143</v>
+      </c>
+      <c r="F83" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>128</v>
+      </c>
+      <c r="B84" t="s">
+        <v>130</v>
+      </c>
+      <c r="C84" t="s">
+        <v>11</v>
+      </c>
+      <c r="D84" t="s">
+        <v>141</v>
+      </c>
+      <c r="E84" t="s">
+        <v>145</v>
+      </c>
+      <c r="F84" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>128</v>
+      </c>
+      <c r="B85" t="s">
+        <v>130</v>
+      </c>
+      <c r="C85" t="s">
+        <v>13</v>
+      </c>
+      <c r="D85" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>128</v>
+      </c>
+      <c r="B86" t="s">
+        <v>130</v>
+      </c>
+      <c r="C86" t="s">
+        <v>13</v>
+      </c>
+      <c r="D86" t="s">
+        <v>188</v>
+      </c>
+      <c r="E86" t="s">
+        <v>147</v>
+      </c>
+      <c r="F86" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>128</v>
+      </c>
+      <c r="B87" t="s">
+        <v>130</v>
+      </c>
+      <c r="C87" t="s">
+        <v>13</v>
+      </c>
+      <c r="D87" t="s">
+        <v>188</v>
+      </c>
+      <c r="E87" t="s">
+        <v>149</v>
+      </c>
+      <c r="F87" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>128</v>
+      </c>
+      <c r="B88" t="s">
+        <v>130</v>
+      </c>
+      <c r="C88" t="s">
+        <v>13</v>
+      </c>
+      <c r="D88" t="s">
+        <v>188</v>
+      </c>
+      <c r="E88" t="s">
+        <v>145</v>
+      </c>
+      <c r="F88" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>128</v>
+      </c>
+      <c r="B89" t="s">
+        <v>130</v>
+      </c>
+      <c r="C89" t="s">
+        <v>152</v>
+      </c>
+      <c r="D89" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>128</v>
+      </c>
+      <c r="B90" t="s">
+        <v>130</v>
+      </c>
+      <c r="C90" t="s">
+        <v>152</v>
+      </c>
+      <c r="D90" t="s">
+        <v>154</v>
+      </c>
+      <c r="E90" t="s">
+        <v>153</v>
+      </c>
+      <c r="F90" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>128</v>
+      </c>
+      <c r="B91" t="s">
+        <v>130</v>
+      </c>
+      <c r="C91" t="s">
+        <v>152</v>
+      </c>
+      <c r="D91" t="s">
+        <v>154</v>
+      </c>
+      <c r="E91" t="s">
+        <v>156</v>
+      </c>
+      <c r="F91" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>128</v>
+      </c>
+      <c r="B92" t="s">
+        <v>130</v>
+      </c>
+      <c r="C92" t="s">
+        <v>152</v>
+      </c>
+      <c r="D92" t="s">
+        <v>154</v>
+      </c>
+      <c r="E92" t="s">
+        <v>129</v>
+      </c>
+      <c r="F92" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>128</v>
+      </c>
+      <c r="B93" t="s">
+        <v>130</v>
+      </c>
+      <c r="C93" t="s">
         <v>159</v>
       </c>
-      <c r="D81" t="s">
+      <c r="D93" t="s">
         <v>173</v>
       </c>
-      <c r="E81" t="s">
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>128</v>
+      </c>
+      <c r="B94" t="s">
+        <v>130</v>
+      </c>
+      <c r="C94" t="s">
+        <v>159</v>
+      </c>
+      <c r="D94" t="s">
+        <v>173</v>
+      </c>
+      <c r="E94" t="s">
+        <v>160</v>
+      </c>
+      <c r="F94" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>128</v>
+      </c>
+      <c r="B95" t="s">
+        <v>130</v>
+      </c>
+      <c r="C95" t="s">
+        <v>159</v>
+      </c>
+      <c r="D95" t="s">
+        <v>173</v>
+      </c>
+      <c r="E95" t="s">
+        <v>162</v>
+      </c>
+      <c r="F95" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>128</v>
+      </c>
+      <c r="B96" t="s">
+        <v>130</v>
+      </c>
+      <c r="C96" t="s">
+        <v>159</v>
+      </c>
+      <c r="D96" t="s">
+        <v>173</v>
+      </c>
+      <c r="E96" t="s">
         <v>164</v>
       </c>
-      <c r="F81" t="s">
+      <c r="F96" t="s">
         <v>165</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Revisions after testing completion
</commit_message>
<xml_diff>
--- a/conf/csvImport/SW Files/SW Files/New Probcodes.xlsx
+++ b/conf/csvImport/SW Files/SW Files/New Probcodes.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27610"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Shared Directory/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Data Files/TOSHIBA EXT/Transfer/EnGee/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -234,9 +234,6 @@
     <t>POW!</t>
   </si>
   <si>
-    <t>POW</t>
-  </si>
-  <si>
     <t>SharePoint Apps</t>
   </si>
   <si>
@@ -604,6 +601,9 @@
   </si>
   <si>
     <t>Network</t>
+  </si>
+  <si>
+    <t>POW0</t>
   </si>
 </sst>
 </file>
@@ -978,8 +978,8 @@
   <dimension ref="A1:F96"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D26" sqref="A1:F96"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -992,22 +992,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B1" t="s">
         <v>166</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>167</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>168</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>169</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>170</v>
-      </c>
-      <c r="F1" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -1015,7 +1015,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -1023,7 +1023,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -1079,7 +1079,7 @@
         <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -1093,7 +1093,7 @@
         <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -1171,7 +1171,7 @@
         <v>20</v>
       </c>
       <c r="D14" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -1199,7 +1199,7 @@
         <v>24</v>
       </c>
       <c r="D16" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -1336,7 +1336,7 @@
         <v>21</v>
       </c>
       <c r="C26" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D26" t="s">
         <v>44</v>
@@ -1549,7 +1549,7 @@
         <v>66</v>
       </c>
       <c r="D38" t="s">
-        <v>67</v>
+        <v>190</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -1560,10 +1560,10 @@
         <v>21</v>
       </c>
       <c r="C39" t="s">
+        <v>67</v>
+      </c>
+      <c r="D39" t="s">
         <v>68</v>
-      </c>
-      <c r="D39" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
@@ -1574,10 +1574,10 @@
         <v>21</v>
       </c>
       <c r="C40" t="s">
+        <v>69</v>
+      </c>
+      <c r="D40" t="s">
         <v>70</v>
-      </c>
-      <c r="D40" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
@@ -1588,10 +1588,10 @@
         <v>21</v>
       </c>
       <c r="C41" t="s">
+        <v>71</v>
+      </c>
+      <c r="D41" t="s">
         <v>72</v>
-      </c>
-      <c r="D41" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
@@ -1602,10 +1602,10 @@
         <v>21</v>
       </c>
       <c r="C42" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D42" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
@@ -1616,10 +1616,10 @@
         <v>21</v>
       </c>
       <c r="C43" t="s">
+        <v>74</v>
+      </c>
+      <c r="D43" t="s">
         <v>75</v>
-      </c>
-      <c r="D43" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
@@ -1630,10 +1630,10 @@
         <v>21</v>
       </c>
       <c r="C44" t="s">
+        <v>76</v>
+      </c>
+      <c r="D44" t="s">
         <v>77</v>
-      </c>
-      <c r="D44" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
@@ -1644,10 +1644,10 @@
         <v>21</v>
       </c>
       <c r="C45" t="s">
+        <v>78</v>
+      </c>
+      <c r="D45" t="s">
         <v>79</v>
-      </c>
-      <c r="D45" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
@@ -1658,10 +1658,10 @@
         <v>21</v>
       </c>
       <c r="C46" t="s">
+        <v>80</v>
+      </c>
+      <c r="D46" t="s">
         <v>81</v>
-      </c>
-      <c r="D46" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
@@ -1672,10 +1672,10 @@
         <v>21</v>
       </c>
       <c r="C47" t="s">
+        <v>82</v>
+      </c>
+      <c r="D47" t="s">
         <v>83</v>
-      </c>
-      <c r="D47" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
@@ -1686,10 +1686,10 @@
         <v>21</v>
       </c>
       <c r="C48" t="s">
+        <v>84</v>
+      </c>
+      <c r="D48" t="s">
         <v>85</v>
-      </c>
-      <c r="D48" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
@@ -1700,800 +1700,800 @@
         <v>21</v>
       </c>
       <c r="C49" t="s">
+        <v>86</v>
+      </c>
+      <c r="D49" t="s">
         <v>87</v>
-      </c>
-      <c r="D49" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B50" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
+        <v>88</v>
+      </c>
+      <c r="B51" t="s">
+        <v>91</v>
+      </c>
+      <c r="C51" t="s">
         <v>89</v>
       </c>
-      <c r="B51" t="s">
+      <c r="D51" t="s">
         <v>92</v>
-      </c>
-      <c r="C51" t="s">
-        <v>90</v>
-      </c>
-      <c r="D51" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
+        <v>88</v>
+      </c>
+      <c r="B52" t="s">
+        <v>91</v>
+      </c>
+      <c r="C52" t="s">
         <v>89</v>
       </c>
-      <c r="B52" t="s">
+      <c r="D52" t="s">
         <v>92</v>
       </c>
-      <c r="C52" t="s">
+      <c r="E52" t="s">
         <v>90</v>
       </c>
-      <c r="D52" t="s">
+      <c r="F52" t="s">
         <v>93</v>
-      </c>
-      <c r="E52" t="s">
-        <v>91</v>
-      </c>
-      <c r="F52" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
+        <v>88</v>
+      </c>
+      <c r="B53" t="s">
+        <v>91</v>
+      </c>
+      <c r="C53" t="s">
         <v>89</v>
       </c>
-      <c r="B53" t="s">
+      <c r="D53" t="s">
         <v>92</v>
       </c>
-      <c r="C53" t="s">
-        <v>90</v>
-      </c>
-      <c r="D53" t="s">
-        <v>93</v>
-      </c>
       <c r="E53" t="s">
+        <v>94</v>
+      </c>
+      <c r="F53" t="s">
         <v>95</v>
-      </c>
-      <c r="F53" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
+        <v>88</v>
+      </c>
+      <c r="B54" t="s">
+        <v>91</v>
+      </c>
+      <c r="C54" t="s">
         <v>89</v>
       </c>
-      <c r="B54" t="s">
+      <c r="D54" t="s">
         <v>92</v>
       </c>
-      <c r="C54" t="s">
-        <v>90</v>
-      </c>
-      <c r="D54" t="s">
-        <v>93</v>
-      </c>
       <c r="E54" t="s">
+        <v>96</v>
+      </c>
+      <c r="F54" t="s">
         <v>97</v>
-      </c>
-      <c r="F54" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B55" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C55" t="s">
+        <v>98</v>
+      </c>
+      <c r="D55" t="s">
         <v>99</v>
-      </c>
-      <c r="D55" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B56" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C56" t="s">
+        <v>100</v>
+      </c>
+      <c r="D56" t="s">
         <v>101</v>
-      </c>
-      <c r="D56" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B57" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C57" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D57" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B58" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C58" t="s">
+        <v>102</v>
+      </c>
+      <c r="D58" t="s">
+        <v>104</v>
+      </c>
+      <c r="E58" t="s">
         <v>103</v>
       </c>
-      <c r="D58" t="s">
-        <v>105</v>
-      </c>
-      <c r="E58" t="s">
-        <v>104</v>
-      </c>
       <c r="F58" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B59" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C59" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D59" t="s">
+        <v>104</v>
+      </c>
+      <c r="E59" t="s">
         <v>105</v>
       </c>
-      <c r="E59" t="s">
-        <v>106</v>
-      </c>
       <c r="F59" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B60" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C60" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D60" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E60" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F60" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B61" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C61" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D61" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E61" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F61" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B62" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C62" t="s">
+        <v>108</v>
+      </c>
+      <c r="D62" t="s">
         <v>109</v>
-      </c>
-      <c r="D62" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B63" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C63" t="s">
+        <v>110</v>
+      </c>
+      <c r="D63" t="s">
         <v>111</v>
-      </c>
-      <c r="D63" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B64" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C64" t="s">
+        <v>112</v>
+      </c>
+      <c r="D64" t="s">
         <v>113</v>
-      </c>
-      <c r="D64" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B65" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C65" t="s">
+        <v>114</v>
+      </c>
+      <c r="D65" t="s">
         <v>115</v>
-      </c>
-      <c r="D65" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B66" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C66" t="s">
+        <v>116</v>
+      </c>
+      <c r="D66" t="s">
         <v>117</v>
-      </c>
-      <c r="D66" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B67" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C67" t="s">
+        <v>118</v>
+      </c>
+      <c r="D67" t="s">
         <v>119</v>
-      </c>
-      <c r="D67" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B68" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C68" t="s">
+        <v>120</v>
+      </c>
+      <c r="D68" t="s">
         <v>121</v>
-      </c>
-      <c r="D68" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B69" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
+        <v>122</v>
+      </c>
+      <c r="B70" t="s">
+        <v>124</v>
+      </c>
+      <c r="C70" t="s">
         <v>123</v>
       </c>
-      <c r="B70" t="s">
+      <c r="D70" t="s">
         <v>125</v>
-      </c>
-      <c r="C70" t="s">
-        <v>124</v>
-      </c>
-      <c r="D70" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B71" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C71" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D71" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B72" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
+        <v>127</v>
+      </c>
+      <c r="B73" t="s">
+        <v>129</v>
+      </c>
+      <c r="C73" t="s">
         <v>128</v>
       </c>
-      <c r="B73" t="s">
-        <v>130</v>
-      </c>
-      <c r="C73" t="s">
-        <v>129</v>
-      </c>
       <c r="D73" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
+        <v>127</v>
+      </c>
+      <c r="B74" t="s">
+        <v>129</v>
+      </c>
+      <c r="C74" t="s">
         <v>128</v>
       </c>
-      <c r="B74" t="s">
+      <c r="D74" t="s">
+        <v>179</v>
+      </c>
+      <c r="E74" t="s">
+        <v>184</v>
+      </c>
+      <c r="F74" t="s">
         <v>130</v>
-      </c>
-      <c r="C74" t="s">
-        <v>129</v>
-      </c>
-      <c r="D74" t="s">
-        <v>180</v>
-      </c>
-      <c r="E74" t="s">
-        <v>185</v>
-      </c>
-      <c r="F74" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B75" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C75" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D75" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B76" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C76" t="s">
+        <v>131</v>
+      </c>
+      <c r="D76" t="s">
+        <v>186</v>
+      </c>
+      <c r="E76" t="s">
+        <v>185</v>
+      </c>
+      <c r="F76" t="s">
         <v>132</v>
-      </c>
-      <c r="D76" t="s">
-        <v>187</v>
-      </c>
-      <c r="E76" t="s">
-        <v>186</v>
-      </c>
-      <c r="F76" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B77" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C77" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D77" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E77" t="s">
+        <v>133</v>
+      </c>
+      <c r="F77" t="s">
         <v>134</v>
-      </c>
-      <c r="F77" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B78" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C78" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D78" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E78" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F78" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B79" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C79" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D79" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E79" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F79" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B80" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C80" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D80" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E80" t="s">
+        <v>137</v>
+      </c>
+      <c r="F80" t="s">
         <v>138</v>
-      </c>
-      <c r="F80" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B81" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C81" t="s">
         <v>11</v>
       </c>
       <c r="D81" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B82" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C82" t="s">
         <v>11</v>
       </c>
       <c r="D82" t="s">
+        <v>140</v>
+      </c>
+      <c r="E82" t="s">
+        <v>139</v>
+      </c>
+      <c r="F82" t="s">
         <v>141</v>
-      </c>
-      <c r="E82" t="s">
-        <v>140</v>
-      </c>
-      <c r="F82" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B83" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C83" t="s">
         <v>11</v>
       </c>
       <c r="D83" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E83" t="s">
+        <v>142</v>
+      </c>
+      <c r="F83" t="s">
         <v>143</v>
-      </c>
-      <c r="F83" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B84" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C84" t="s">
         <v>11</v>
       </c>
       <c r="D84" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E84" t="s">
+        <v>144</v>
+      </c>
+      <c r="F84" t="s">
         <v>145</v>
-      </c>
-      <c r="F84" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B85" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C85" t="s">
         <v>13</v>
       </c>
       <c r="D85" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B86" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C86" t="s">
         <v>13</v>
       </c>
       <c r="D86" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E86" t="s">
+        <v>146</v>
+      </c>
+      <c r="F86" t="s">
         <v>147</v>
-      </c>
-      <c r="F86" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B87" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C87" t="s">
         <v>13</v>
       </c>
       <c r="D87" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E87" t="s">
+        <v>148</v>
+      </c>
+      <c r="F87" t="s">
         <v>149</v>
-      </c>
-      <c r="F87" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B88" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C88" t="s">
         <v>13</v>
       </c>
       <c r="D88" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E88" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F88" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B89" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C89" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D89" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B90" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C90" t="s">
+        <v>151</v>
+      </c>
+      <c r="D90" t="s">
+        <v>153</v>
+      </c>
+      <c r="E90" t="s">
         <v>152</v>
       </c>
-      <c r="D90" t="s">
+      <c r="F90" t="s">
         <v>154</v>
-      </c>
-      <c r="E90" t="s">
-        <v>153</v>
-      </c>
-      <c r="F90" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B91" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C91" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D91" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E91" t="s">
+        <v>155</v>
+      </c>
+      <c r="F91" t="s">
         <v>156</v>
-      </c>
-      <c r="F91" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
+        <v>127</v>
+      </c>
+      <c r="B92" t="s">
+        <v>129</v>
+      </c>
+      <c r="C92" t="s">
+        <v>151</v>
+      </c>
+      <c r="D92" t="s">
+        <v>153</v>
+      </c>
+      <c r="E92" t="s">
         <v>128</v>
       </c>
-      <c r="B92" t="s">
-        <v>130</v>
-      </c>
-      <c r="C92" t="s">
-        <v>152</v>
-      </c>
-      <c r="D92" t="s">
-        <v>154</v>
-      </c>
-      <c r="E92" t="s">
-        <v>129</v>
-      </c>
       <c r="F92" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B93" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C93" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D93" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B94" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C94" t="s">
+        <v>158</v>
+      </c>
+      <c r="D94" t="s">
+        <v>172</v>
+      </c>
+      <c r="E94" t="s">
         <v>159</v>
       </c>
-      <c r="D94" t="s">
-        <v>173</v>
-      </c>
-      <c r="E94" t="s">
+      <c r="F94" t="s">
         <v>160</v>
-      </c>
-      <c r="F94" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B95" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C95" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D95" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E95" t="s">
+        <v>161</v>
+      </c>
+      <c r="F95" t="s">
         <v>162</v>
-      </c>
-      <c r="F95" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B96" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C96" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D96" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E96" t="s">
+        <v>163</v>
+      </c>
+      <c r="F96" t="s">
         <v>164</v>
-      </c>
-      <c r="F96" t="s">
-        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -2513,7 +2513,7 @@
   <sheetData>
     <row r="1" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I1">
         <f>COUNTIF(H1:H32,H1)</f>
@@ -2522,7 +2522,7 @@
     </row>
     <row r="2" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I2">
         <f t="shared" ref="I2:I32" si="0">COUNTIF(H2:H33,H2)</f>
@@ -2531,7 +2531,7 @@
     </row>
     <row r="3" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I3">
         <f t="shared" si="0"/>
@@ -2540,7 +2540,7 @@
     </row>
     <row r="4" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I4">
         <f t="shared" si="0"/>
@@ -2549,7 +2549,7 @@
     </row>
     <row r="5" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I5">
         <f t="shared" si="0"/>
@@ -2558,7 +2558,7 @@
     </row>
     <row r="6" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I6">
         <f t="shared" si="0"/>
@@ -2567,7 +2567,7 @@
     </row>
     <row r="7" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I7">
         <f t="shared" si="0"/>
@@ -2585,7 +2585,7 @@
     </row>
     <row r="9" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I9">
         <f t="shared" si="0"/>
@@ -2594,7 +2594,7 @@
     </row>
     <row r="10" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I10">
         <f t="shared" si="0"/>
@@ -2603,7 +2603,7 @@
     </row>
     <row r="11" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I11">
         <f t="shared" si="0"/>
@@ -2612,7 +2612,7 @@
     </row>
     <row r="12" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I12">
         <f t="shared" si="0"/>
@@ -2621,7 +2621,7 @@
     </row>
     <row r="13" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I13">
         <f t="shared" si="0"/>
@@ -2630,7 +2630,7 @@
     </row>
     <row r="14" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H14" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I14">
         <f t="shared" si="0"/>
@@ -2639,7 +2639,7 @@
     </row>
     <row r="15" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I15">
         <f t="shared" si="0"/>
@@ -2648,7 +2648,7 @@
     </row>
     <row r="16" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H16" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I16">
         <f t="shared" si="0"/>
@@ -2657,7 +2657,7 @@
     </row>
     <row r="17" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I17">
         <f t="shared" si="0"/>
@@ -2684,7 +2684,7 @@
     </row>
     <row r="20" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I20">
         <f t="shared" si="0"/>
@@ -2693,7 +2693,7 @@
     </row>
     <row r="21" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I21">
         <f t="shared" si="0"/>
@@ -2702,7 +2702,7 @@
     </row>
     <row r="22" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H22" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I22">
         <f t="shared" si="0"/>
@@ -2729,7 +2729,7 @@
     </row>
     <row r="25" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I25">
         <f t="shared" si="0"/>
@@ -2747,7 +2747,7 @@
     </row>
     <row r="27" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H27" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I27">
         <f t="shared" si="0"/>
@@ -2756,7 +2756,7 @@
     </row>
     <row r="28" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H28" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I28">
         <f t="shared" si="0"/>
@@ -2765,7 +2765,7 @@
     </row>
     <row r="29" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H29" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I29">
         <f t="shared" si="0"/>
@@ -2774,7 +2774,7 @@
     </row>
     <row r="30" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H30" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I30">
         <f t="shared" si="0"/>
@@ -2783,7 +2783,7 @@
     </row>
     <row r="31" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H31" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I31">
         <f t="shared" si="0"/>

</xml_diff>